<commit_message>
[SHUBHAM] Adding updated code
</commit_message>
<xml_diff>
--- a/data/excel/goNowFlight+Hotel.xlsx
+++ b/data/excel/goNowFlight+Hotel.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\GoNow\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72B5A4F-DBCC-4225-BB3F-69B2CC130D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="139">
   <si>
     <t>UserType</t>
   </si>
@@ -424,12 +424,30 @@
   </si>
   <si>
     <t>78AJI0321K,897NKJ233G</t>
+  </si>
+  <si>
+    <t>10,November 2023</t>
+  </si>
+  <si>
+    <t>15,November 2023</t>
+  </si>
+  <si>
+    <t>//www.gonowtravel.com.au/</t>
+  </si>
+  <si>
+    <t>Delhi, India - Indira Gandhi Int'l Airport (DEL)</t>
+  </si>
+  <si>
+    <t>maa</t>
+  </si>
+  <si>
+    <t>Chennai, India - Chennai (MAA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -564,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -595,6 +613,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -875,11 +894,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4351BBB2-D99B-4FE0-BCDE-021161669266}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
-      <selection activeCell="BR9" sqref="BR9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,47 +1612,810 @@
     </row>
   </sheetData>
   <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V3" xr:uid="{B3BA032E-3D34-4541-B546-CA6851BCBAF8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V3">
       <formula1>"Economy,Premium Economy,Business,First Class"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S3 W2:X3 AA2:AA3 AE2:AF3" xr:uid="{437DB5DD-A848-4921-AFFD-57D2E902BF14}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S3 W2:X3 AA2:AA3 AE2:AF3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3" xr:uid="{FE7092E2-A1A7-4C65-9F0E-9EE93B3576D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3">
       <formula1>"LogIn,Guest"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB3" xr:uid="{D41E9235-2320-47DE-A595-6B72FA896A89}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB3">
       <formula1>"All,1 StarAndAbove,2 StarAndAbove,3 StarAndAbove,4 StarAndAbove,5 Star,NotRatedStar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC3" xr:uid="{F437B87F-A249-4447-AB27-1D31F83362C1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC3">
       <formula1>"All,Hotel,Apartment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD3" xr:uid="{DE125D7B-8901-4C46-B1AE-6524C33D2185}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD3">
       <formula1>"All,RoomRate,PackageRate"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG3" xr:uid="{E9C9C38A-909B-4447-9D38-86C762A5D6E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG3">
       <formula1>"Refundable,Non-Refundable,All"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2:BJ3" xr:uid="{19036A71-D133-4362-AAC9-C64FA532636B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2:BJ3">
       <formula1>"5123456789012346,4111111111111111"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI3" xr:uid="{BBAF6A79-2E1A-4FA9-A0F3-9471ADFEFC86}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI3">
       <formula1>"Master Card,Visa"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3" xr:uid="{3623F404-8488-4F9E-BB42-9EB9D2AFF4BE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
       <formula1>"AUD,USD,AED,INR,EUR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{0B9BDCA2-31F8-4682-93B2-B1C2C0ADBE50}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="AI2" r:id="rId1" xr:uid="{4DA62A0A-4D51-4CC2-AF7A-D34D901917B1}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{497D44C7-2588-4F1E-9213-8DD8A3D7D57E}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{B856A042-23DE-4425-AEBE-6570288C02C8}"/>
-    <hyperlink ref="AI3" r:id="rId4" xr:uid="{65907A78-CAA6-464D-B8E0-8C78EFD403BE}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{4F9FE738-9112-40A8-936C-3E8A3945F91C}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{68C696C6-E325-4E17-99C2-A354CFADA882}"/>
+    <hyperlink ref="AI2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="AI3" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BR3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="35" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="36" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="16" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BI1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="BJ1" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="BN1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="BO1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BQ1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="BR1" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="3">
+        <v>2</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>8447422233</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU2" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="BE2" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="BF2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="BH2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BJ2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM2" s="3">
+        <v>123</v>
+      </c>
+      <c r="BN2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="BO2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="BP2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR2" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="3">
+        <v>2</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL3" s="3">
+        <v>8447422233</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS3" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="AT3" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU3" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="BB3" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC3" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="BE3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="BF3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="BG3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="BH3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="BI3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BJ3" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="BK3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BL3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BM3" s="3">
+        <v>123</v>
+      </c>
+      <c r="BN3" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="BO3" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="BP3" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="BQ3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR3" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
+      <formula1>"Domestic,International"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
+      <formula1>"AUD,USD,AED,INR,EUR"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2:BI3">
+      <formula1>"Master Card,Visa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2:BJ3">
+      <formula1>"5123456789012346,4111111111111111"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2:AG3">
+      <formula1>"Refundable,Non-Refundable,All"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD3">
+      <formula1>"All,RoomRate,PackageRate"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC3">
+      <formula1>"All,Hotel,Apartment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB3">
+      <formula1>"All,1 StarAndAbove,2 StarAndAbove,3 StarAndAbove,4 StarAndAbove,5 Star,NotRatedStar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3">
+      <formula1>"LogIn,Guest"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S3 W2:X3 AA2:AA3 AE2:AF3">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V3">
+      <formula1>"Economy,Premium Economy,Business,First Class"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AI2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="AI3" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>